<commit_message>
one of last commit
</commit_message>
<xml_diff>
--- a/src/openai/Olbia_text/responses/mini_1/temp_1.0/DET_DETE_345_2025-response.xlsx
+++ b/src/openai/Olbia_text/responses/mini_1/temp_1.0/DET_DETE_345_2025-response.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -453,13 +453,13 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Intestazione: Settore, Servizio e Autorità che emana il provvedimento e tipo di provvedimento.</t>
+          <t>Intestazione: Settore, Servizio e Autorità che emana il provvedimento e tipo di provvedimento. Nella determina oltre il settore va indicato il servizio di appartenenza presente nella macrostruttura vigente.</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>RISPOSTA: NO
-Note: Nella determina non è specificato il servizio di appartenenza presente nella macrostruttura vigente.</t>
+Note: Non è esplicitato nella determina il servizio di appartenenza presente nella macrostruttura vigente.</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -476,19 +476,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : NO
+Note: L’oggetto della determinazione menziona il codice 15275 anziché 15271, è necessario correggerlo.</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Indicazione del CIG, del CPV e del CUP (l’indicazione del CUI:  non è richiesta per gli affidamenti diretti ai sensi dell’art. 50 del Dlgs n.36/2023, in quanto consentiti per importi per i quali non è dovuto l’inserimento nei programmi triennali. È richiesta per affidamenti diretti ai sensi dell’art.76 del Dlgs n.36/2023. In caso di consegne complementari ex art.76, comma 4, let. B, o di ripetizione di lavori o servizi analoghi ex art. 76, comma 6, dovrà essere indicato il CUI dell’appalto principale del quale l’affidamento diretto risulta complementare o analogo)</t>
+          <t>Indicazione del CIG e /o del CUP del CUI, del CPV</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -522,12 +523,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Estremi decreto sindacale di nomina del Dirigente.</t>
+          <t>Estremi decreto sindacale di nomina del dirigente.</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -539,46 +540,47 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Conflitto d’interessi</t>
+          <t>Estremi della delega alla firma dell'atto, se persona diversa dal Dirigente.</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA: NO</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Estremi della delega alla firma dell’atto, se persona diversa dal Dirigente.</t>
+          <t>Estremi atto di nomina del Responsabile del Progetto.</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Estremi atto di nomina del Responsabile unico del Progetto, se nominato.</t>
+          <t xml:space="preserve">Conflitto d'interessi </t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA: SI
+Nota: La determina menziona che non sussistono situazioni di conflitto di interessi in relazione ai soggetti coinvolti nella procedura, in conformità all'art. 16 del D.lgs. n. 36/2023.</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -590,7 +592,13 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Normativa specifica:  Codice dei contratti pubblici (D.Lgs. n. 36.2023.) ;  L. R. n. 8/2018;  Art. 26 legge n.488/1999  Art. 1, D.L. 6 luglio 2012 n. 95 convertito dalla legge 7 agosto 2012 n. 135 (adesione convenzione Consip e MEPA);  Art. 1, comma 450, della legge 27 Dicembre 2006, n. 296 e ss.mm.ii. (per quanto applicabile);  Art. 26, della legge n. 488/1999 e ss.mm.ii.; DPCM 24 dicembre 2015 ;</t>
+          <t>**Normativa specifica**:
+Codice dei contratti pubblici (D.Lgs. n. 36.2023.);
+L.R. n. 8/2018 e ss.mm.ii. (per quanto applicabile);
+Art. 1, D.L. 6 luglio 2012 n. 95 convertito dalla legge 7 agosto 2012, n. 135 (adesione convenzione Consip);
+Art. 1, comma 450, della legge 27 Dicembre 2006, n. 296 e ss.mm.ii. (per quanto applicabile);
+Art. 26, della legge n. 488/1999 e ss.mm.ii.;
+DPCM 24 dicembre 2015.</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -607,12 +615,18 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Normativa generale:  TUEL;  Legge n. 241/90;  DPR n. 62/2013 Codice comportamento dipendenti pubblici;  L. n. 190/2012;  D.Lgs. n. 33/2013.  Legge n° 136/2010</t>
+          <t>**Normativa generale**:
+TUEL;
+Legge n. 241/90;
+DPR n. 62/2013 Codice comportamento dipendenti pubblici;
+L. n. 190/2012;
+D.Lgs. n. 33/2013;
+Legge n.136/2010.</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -624,30 +638,34 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Norme di principio   Art. 4 del Dlgs n.36/2023. (Criterio interpretativo e applicativo)</t>
+          <t>**Norme di principio**
+Art. 4 del Dlgs n.36/2023. (Criterio interpretativo e applicativo)</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>RISPOSTA : SI</t>
+          <t>RISPOSTA : NO</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Regolamenti dell’ente quali:  - Statuto Comunale;  - Regolamento di contabilità;  - Regolamento dei contratti</t>
+          <t>Regolamenti dell’ente quali:
+- Statuto Comunale;
+- Regolamento di contabilità;
+- Regolamento dei contratti</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>RISPOSTA: NO
-Note: Non è menzionato né lo Statuto Comunale, né il Regolamento di contabilità, né il Regolamento dei contratti nella determina.</t>
+Note: Nella determina non si fa esplicito riferimento allo Statuto Comunale, al Regolamento di contabilità, né al Regolamento dei contratti.</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -659,47 +677,48 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Indicazione dei riferimenti della determina a contrarre “semplificata” adottata</t>
+          <t xml:space="preserve">Termini per la conclusione della procedura </t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>RISPOSTA: YES</t>
+          <t>RISPOSTA: NO
+Note: Non è presente alcun riferimento ai termini per la conclusione della procedura nella determina.</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Indicazione dei riferimenti della determina a contrarre “non semplificata” adottata</t>
+          <t>Fine che con il contratto si intende perseguire</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Note: La determina non riporta esplicitamente l'indicazione dei riferimenti della determina a contrarre "non semplificata".</t>
+          <t>RISPOSTA: SI</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Elementi da approvare con la determina a contrarre nel caso di provvedimento unico</t>
+          <t>Oggetto del contratto</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>RISPOSTA: NO 
+Note: La determina non specifica un capitolato d’appalto, quaderno d’oneri o schema di contratto.</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -711,7 +730,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Per gli appalti di servizi: DUVRI</t>
+          <t>DUVRI (per i servizi)</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -728,13 +747,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Suddivisione in lotti e norme sull’indebito frazionamento</t>
+          <t xml:space="preserve">Costo della mano d’opera; contratto applicabile </t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO  
-Note: Nella determina non è presente alcun riferimento alla mancata suddivisione dell'appalto in lotti, né motivazioni correlate al rispetto dell'art. 58 del Dlgs n. 36/2023.</t>
+          <t>NO</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -746,13 +764,13 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Validazione (in caso di lavori pubblici)</t>
+          <t>Suddivisione in lotti</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>RISPOSTA : NO
-Note: Non è stata fornita alcuna indicazione riguardo all'avvenuta validazione del progetto posto a base di gara.</t>
+Nota: La determina non menziona la motivazione sulla mancata suddivisione dell'appalto in lotti ai sensi dell’art. 58 del Dlgs n. 36/2023.</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -764,12 +782,13 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Criteri Ambientali Minimi (CAM)</t>
+          <t>Validazione (in caso di lavori pubblici)</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO</t>
+          <t>RISPOSTA : NO
+Note: Nel testo della determina non è menzionata la validazione del progetto posto a base di gara.</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -781,12 +800,13 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Cauzione</t>
+          <t>Criteri Ambientali minimi</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO</t>
+          <t>RISPOSTA: NO
+Note: Nella determina non è presente alcun riferimento ai Criteri Ambientali Minimi (CAM) o alla loro applicazione.</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -798,13 +818,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Riferimenti all’obbligo di utilizzo di convenzioni Consip o di soggetti aggregatori</t>
+          <t>Forma del contratto</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI
-Note: Nella determina si fa riferimento alla verifica che non ci siano convenzioni attive di Consip o di altro soggetto aggregatore relative alla fornitura oggetto dell'affidamento, quindi è stato giustificato il ricorso all'affidamento diretto.</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -816,30 +835,30 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Riferimenti all’obbligo di utilizzo del MEPA o del sistema telematico messo a disposizione dalla centrale regionale di riferimento</t>
+          <t>Clausole del contratto ritenute essenziali</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Note: Nella determina è specificato che l'importo dell'affidamento è di € 4.026,00, quindi è superiore alla soglia di € 5.000,00, e infatti viene fatto ricorso al MEPA. Tuttavia, non è menzionato un riferimento diretto all'obbligo di utilizzo del MEPA in ottemperanza all'art. 1, comma 449 della legge 296/2006.</t>
+          <t>RISPOSTA: SI</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Indicazioni in merito all’istruttoria propedeutica al provvedimento</t>
+          <t>Cauzione provvisoria</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO</t>
+          <t>RISPOSTA: NO
+Note: Non viene richiesta la garanzia definitiva in quanto l’affidamento non lo prevede, secondo quanto indicato nella determina.</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -851,13 +870,13 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Denominazione dell’operatore economico affidatario e indicazione relativa all’acquisizione dell’offerta</t>
+          <t>Modalità di scelta del contraente e ragioni che ne sono alla base (motivare in modo specifico) e criteri di selezione delle offerte</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO  
-Note: La determina non riporta la denominazione dell’operatore economico affidatario e l'indicazione relativa all'acquisizione dell'offerta.</t>
+          <t>RISPOSTA: NO
+Note: La determina non fornisce una motivazione specifica riguardante la modalità di scelta del contraente e i criteri di selezione delle offerte, come richiesto dal punto 24.</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -869,13 +888,13 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Importo di affidamento</t>
+          <t xml:space="preserve">Rotazione degli affidamenti </t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Note: Non ci sono riferimenti specifici all'importo di affidamento e agli eventuali oneri della sicurezza, oneri interferenziali, costo della manodopera, contratto collettivo di lavoro applicato, quinto d’obbligo, revisione dei prezzi, somme a disposizione, supporto al RUP e incentivi nel testo della determinazione.</t>
+          <t>RISPOSTA : NO
+Note: La determina specifica che il principio di rotazione di cui all’art. 49 del d.lgs. 36/2023 può essere derogato per gli affidamenti diretti di importo inferiore a 5.000 euro. Questo implica che non si applica la rotazione per la presente procedura.</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -887,47 +906,50 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Indicazione di requisiti previsti dalle disposizioni vigenti per il ricorso all’affidamento diretto.</t>
+          <t>Indicazione dell’importo massimo stimato a base di gara
+Quadro economico dell’intervento  comprensivo di 
+Importo a base di gara, oneri fiscali, costi della sicurezza/interferenziali, revisione dei prezzi, somme a disposizione, supporto al RUP, incentivi (art. 45) modificazioni del contratto preventivabili, proroga, lavori o servizi analoghi, quinto d’obbligo</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA: NO
+Nota: Nella determina non è presente un'indicazione chiara dell'importo massimo stimato a base di gara e del quadro economico dell'intervento, come i costi della sicurezza, oneri fiscali, e altre voci richieste. Questo rappresenta una grave omissione.</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Motivazione scelta della procedura e del contraente;        Esporre le ragioni della scelta della ditta affidataria;        Esposizione del fatto che legittima il ricorso alla procedura e della valutazione in ordine alla scelta del contraente.</t>
+          <t xml:space="preserve">Riferimenti all’obbligo di utilizzo degli strumenti di acquisto e di negoziazione messi a disposizione da CONSIP e da soggetti aggregatori </t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : NO
+Note: La determina non menziona chiaramente il rispetto degli obblighi di utilizzo degli strumenti di acquisto e di negoziazione messi a disposizione da CONSIP e da soggetti aggregatori, come richiesto.</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Motivazione scelta della procedura nel caso di ricorso all’art. 76, del Dlgs n.36/2023</t>
+          <t>Riferimenti alla qualificazione del Comune quale Stazione appaltante</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Nota: Non viene fornita una motivazione specifica per il ricorso alla procedura ex art. 76, del D.lgs. n. 36/2023.</t>
+          <t>RISPOSTA : NO</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -939,30 +961,30 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Conformità dell’affidamento ai principi ed alle norme in materia di appalti pubblici</t>
+          <t>Riferimenti alla deliberazione di approvazione del bilancio.</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>RISPOSTA : SI</t>
+          <t>RISPOSTA: NO
+Note: Non sono presenti riferimenti alla deliberazione di approvazione del bilancio pluriennale vigente nella determina.</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>NO</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Dare atto della verifica dei requisiti dell’affidatario</t>
+          <t>Riferimenti deliberazione approvazione PEG e del PIAO</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Nota: Non si trova menzione esplicita della verifica dei requisiti dell'affidatario nella determina.</t>
+          <t>RISPOSTA : NO</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -974,12 +996,13 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Verifica sulla regolarità contributiva, DURC o attestazione della stessa o autocertificazione (limitata ai casi previsti dalla legge).</t>
+          <t>Impegno di spesa/prenotazione/copertura finanziaria</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : SI 
+Nota: L'importo da impegnare è di € 4.026,00, assoggettato a IVA al 22% per una parte (aggiornamento Software Auditing PA) mentre la formazione è esente da IVA ai sensi dell’articolo 10, primo comma, n. 20) del D.P.R. 633/72. Non ci sono riferimenti a bilancio e PEG non approvati o impegni di spesa pluriennali nel testo della determina.</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -991,31 +1014,29 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Riferimenti alla deliberazione di approvazione del bilancio.</t>
+          <t>Conformità dei pagamenti con le regole della finanza pubblica vigenti.</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO
-Note: Nella determina non sono stati indicati gli estremi di approvazione del bilancio pluriennale vigente.</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Riferimenti deliberazione approvazione PEG e al PIAO</t>
+          <t>Contributo ANAC</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>RISPOSTA: NO 
-Note: Nella determina non sono presenti riferimenti alla deliberazione di approvazione del Piano Esecutivo di Gestione (PEG) o al Piano Integrato di Attività e Organizzazione (PIAO).</t>
+          <t>RISPOSTA : NO</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1027,12 +1048,12 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Impegno di spesa/prenotazione</t>
+          <t>Richiamati e/o allegati</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>RISPOSTA: SI</t>
+          <t>RISPOSTA : SI</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
@@ -1044,43 +1065,41 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Contributo ANAC</t>
+          <t>Obblighi di pubblicità e trasparenza</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO
-Note: Non è menzionato né assunto un impegno di spesa relativo al pagamento del contributo all'ANAC nella determina.</t>
+          <t>RISPOSTA: SI</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Flussi finanziari</t>
+          <t>Pubblicazione atti all’Albo Pretorio Online</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>RISPOSTA : NO
-Nota: La determina non contiene riferimenti specifici all'obbligo di tracciabilità dei flussi finanziari ai sensi della legge n° 136/2010 nel contesto indicato.</t>
+          <t>RISPOSTA: SI</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Conformità dei pagamenti con le regole della finanza pubblica vigenti</t>
+          <t>Acquisizione del visto di regolarità contabile ai sensi dell’art. 153 del D.Lgs. n. 267/2000</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1097,155 +1116,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Indicazione esatta dell’aggiudicatario: nome, cognome, ragione sociale, indirizzo, P.Iva, Cod. Fiscale, sede legale/operativa, altro.</t>
+          <t>Sottoscrizione del Dirigente firmatario dell’atto e dove previsto del R.P. o RUP.</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>RISPOSTA : SI</t>
+          <t>RISPOSTA: SI</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
           <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Comunicazione all’aggiudicatario dell’impegno di spesa, la copertura finanziaria, CIG</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>RISPOSTA: SI</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Indicazione specifica della tipologia del contratto</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>RISPOSTA : SI</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Obblighi di pubblicità e trasparenza</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>RISPOSTA: SI</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Attestazione circa il rispetto delle prescrizioni del   PTPCT dell’Ente</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>RISPOSTA: NO
-Note: Non è presente l'attestazione circa il rispetto delle prescrizioni del PTPCT dell'Ente.</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>NO</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Pubblicazione atti all’Albo Pretorio Online.</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>RISPOSTA: SI</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Indicazione termini e autorità a cui ricorrere</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>RISPOSTA: SI</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Sottoscrizione del Dirigente firmatario dell’atto e, dove previsto, del RP o RUP.</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>RISPOSTA: SI</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>SI</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Presenza del visto di regolarità contabile</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>RISPOSTA: NO
-Note: Non risulta presente il visto di regolarità contabile nella determina.</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>NO</t>
         </is>
       </c>
     </row>

</xml_diff>